<commit_message>
20200403{Start a new day}
</commit_message>
<xml_diff>
--- a/2020/3.xlsx
+++ b/2020/3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44CFF1-C019-4003-85A8-03810A0CB956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CACEEE7-1E7A-4A8B-8D52-50E44DFF1128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69693E65-AD6F-44D6-B0ED-1B386BB2E7FA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t xml:space="preserve">Mahabah </t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>1=27</t>
+  </si>
+  <si>
+    <t>Lecture 4 Data Mining</t>
+  </si>
+  <si>
+    <t>10:50 =&gt; 12:00</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -130,6 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
@@ -445,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA183D7-129D-4FE3-AEAC-265A19317476}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +472,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +485,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -486,8 +502,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>8</v>
@@ -496,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>10</v>
@@ -505,7 +524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>13</v>
@@ -514,10 +533,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
   </sheetData>

</xml_diff>